<commit_message>
added relations between drugs and targets to cido
merged dron drug target relations to cido
</commit_message>
<xml_diff>
--- a/src/ontology/Ontorat input/DRON drug_target rat files/DRON_drug_target_antagonist.xlsx
+++ b/src/ontology/Ontorat input/DRON drug_target rat files/DRON_drug_target_antagonist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_yin\Dropbox\Coronavirus drug paper prep\Yingtong Data\DRON drug_target rat files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e342ab95cc976646/文档/GitHub/cido/src/ontology/Ontorat input/DRON drug_target rat files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04562412-04F0-40A2-8C8A-794242112ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{04562412-04F0-40A2-8C8A-794242112ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17A86CB0-4D91-4F88-B88B-B9C5420AAD0F}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="7098" windowWidth="10566" windowHeight="5880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -812,14 +812,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="18.734375" customWidth="1"/>
     <col min="2" max="2" width="13.1015625" customWidth="1"/>
     <col min="3" max="3" width="20.41796875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>